<commit_message>
generate requirements and coverage csv using new tools
</commit_message>
<xml_diff>
--- a/lib/subscriptions_test_kit/requirements/hl7.fhir.uv.subscriptions_1.1.0_requirements.xlsx
+++ b/lib/subscriptions_test_kit/requirements/hl7.fhir.uv.subscriptions_1.1.0_requirements.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/knaden/Documents/Inferno/source/subscriptions-test-kit/lib/subscriptions_test_kit/requirements/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4CEA1058-2D0E-3A4A-945B-153E0EDCE66E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{358A0A83-AEA2-0A40-82FF-43B28935F773}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="19980" firstSheet="1" activeTab="1" xr2:uid="{D251129A-65BB-5042-909C-749E11B8C0B0}"/>
   </bookViews>
@@ -138,7 +138,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1818" uniqueCount="693">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1822" uniqueCount="697">
   <si>
     <r>
       <rPr>
@@ -3695,6 +3695,18 @@
   <si>
     <t xml:space="preserve"> - - Group: Error Handling and Recovery</t>
   </si>
+  <si>
+    <t>Id</t>
+  </si>
+  <si>
+    <t>hl7.fhir.uv.subscriptions_1.1.0</t>
+  </si>
+  <si>
+    <t>Subscriptions R5 Backport IG</t>
+  </si>
+  <si>
+    <t>https://hl7.org/fhir/uv/subscriptions-backport/STU1.1/</t>
+  </si>
 </sst>
 </file>
 
@@ -4100,7 +4112,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="58">
+  <cellXfs count="59">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -4239,6 +4251,7 @@
     <xf numFmtId="0" fontId="5" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -4670,7 +4683,7 @@
       <pane xSplit="5" ySplit="1" topLeftCell="U2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="K137" sqref="K137:K139"/>
+      <selection pane="bottomRight" activeCell="V4" sqref="V4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -13726,10 +13739,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C323F474-BE25-4449-9222-E1A46A1843B5}">
-  <dimension ref="A1:B14"/>
+  <dimension ref="A1:B15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -13750,61 +13763,75 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" s="22" t="s">
-        <v>517</v>
+        <v>693</v>
+      </c>
+      <c r="B3" s="23" t="s">
+        <v>694</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" s="22" t="s">
-        <v>518</v>
+        <v>517</v>
+      </c>
+      <c r="B4" s="58" t="s">
+        <v>696</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" s="22" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" s="22" t="s">
-        <v>520</v>
+        <v>519</v>
+      </c>
+      <c r="B6" s="23" t="s">
+        <v>695</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" s="22" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" s="22" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" s="22" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" s="22" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" s="22" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12" s="22" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13" s="22" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14" s="22" t="s">
+        <v>527</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A15" s="22" t="s">
         <v>528</v>
       </c>
     </row>
@@ -13812,7 +13839,11 @@
   <mergeCells count="1">
     <mergeCell ref="A1:B2"/>
   </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="B4" r:id="rId1" xr:uid="{F5432317-EC62-D640-AC64-C6FD80119192}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 

</xml_diff>